<commit_message>
created records for composition and provided in a separate sheet
</commit_message>
<xml_diff>
--- a/excel_automation/template_project_parameters_all_fields.xlsx
+++ b/excel_automation/template_project_parameters_all_fields.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Orçamento" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Composições" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t xml:space="preserve">Planilha de Orçamento SINTÉTICA</t>
   </si>
@@ -213,6 +214,51 @@
   <si>
     <t xml:space="preserve">bom_name</t>
   </si>
+  <si>
+    <t xml:space="preserve">COMPOSIÇÕES DE CUSTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPOSIÇÃO DE CUSTO UNITÁRIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comp_proj_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comp_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comp_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comp_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrição dos serviços</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R$ Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R$ Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bom_quant_avgprice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL MATERIAL/EQUIPAMENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all_total</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +274,7 @@
     <numFmt numFmtId="170" formatCode="000,000.00"/>
     <numFmt numFmtId="171" formatCode="0,000,000.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -324,6 +370,40 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="17"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF31708F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -390,7 +470,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -519,6 +599,26 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +644,7 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF31708F"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
@@ -599,8 +699,8 @@
   </sheetPr>
   <dimension ref="A1:N236"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="F3 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3857,4 +3957,110 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.04"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D8" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>